<commit_message>
Add retrieve cell value from another sheet
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Hello World</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Click here to go to Google</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
   <si>
     <t>The following cell will be modified later</t>
@@ -786,7 +789,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -795,6 +798,14 @@
     <row r="1">
       <c r="A1" t="s" s="0">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>
@@ -815,10 +826,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>